<commit_message>
set up example data
</commit_message>
<xml_diff>
--- a/docs/data-raw/participant_demo.xlsx
+++ b/docs/data-raw/participant_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnfranchak/Documents/GitHub-259-2022/259-exploratory-data-analysis/docs/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223492F-6B55-3B41-BCA5-D48F43356049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307ED894-BCF6-624F-97FF-BBA1F9E28DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16940" yWindow="5260" windowWidth="40000" windowHeight="28320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="65">
   <si>
     <t>Rectangle</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>corrected (contacts)</t>
-  </si>
-  <si>
-    <t>11/18/200</t>
   </si>
   <si>
     <t>asian</t>
@@ -1251,7 +1248,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,16 +1281,16 @@
         <v>36</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>38</v>
@@ -1770,14 +1767,14 @@
       <c r="D14" s="8">
         <v>18</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="12">
+        <v>36848</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>47</v>
@@ -1786,7 +1783,7 @@
         <v>28</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="14"/>
@@ -1814,7 +1811,7 @@
         <v>42</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="36" t="s">
         <v>21</v>
@@ -1921,7 +1918,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="36" t="s">
         <v>11</v>
@@ -1959,7 +1956,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="36" t="s">
         <v>20</v>
@@ -2065,7 +2062,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" s="36" t="s">
         <v>11</v>
@@ -2074,7 +2071,7 @@
         <v>5</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K22" s="8">
         <v>74</v>
@@ -2253,7 +2250,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H27" s="54" t="s">
         <v>11</v>
@@ -2294,7 +2291,7 @@
         <v>42</v>
       </c>
       <c r="H28" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I28" s="36" t="s">
         <v>48</v>

</xml_diff>